<commit_message>
Completed data for Estonia (for now)
</commit_message>
<xml_diff>
--- a/raw data/Lines.xlsx
+++ b/raw data/Lines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\web-projects\baltic-rails-leaflet\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D8378-F4F0-44F4-BB89-4A88C13F710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531C523E-1706-48B4-8166-35065DA6D67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="107">
   <si>
     <t>Line ID</t>
   </si>
@@ -330,6 +330,30 @@
   </si>
   <si>
     <t>Southern section rebuilt</t>
+  </si>
+  <si>
+    <t>Türi—Paide—Tamsalu</t>
+  </si>
+  <si>
+    <t>Extension to Tamsalu built 1915</t>
+  </si>
+  <si>
+    <t>Narva—Musta</t>
+  </si>
+  <si>
+    <t>Rail line between Auvere and power plant dismantled</t>
+  </si>
+  <si>
+    <t>Sonda—Mustvee</t>
+  </si>
+  <si>
+    <t>~2km rebuilt as a museum railway</t>
+  </si>
+  <si>
+    <t>Rakvere—Kunda</t>
+  </si>
+  <si>
+    <t>Tallinn—Narva</t>
   </si>
 </sst>
 </file>
@@ -591,10 +615,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1966,6 +1990,130 @@
         <v>0</v>
       </c>
     </row>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>40</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1900</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1972</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H55" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>41</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1969</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="1">
+        <v>2001</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>42</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1926</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1973</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1870</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H58" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>110</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1870</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H59" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>